<commit_message>
07/03/2023 -> Scripting DPLKKEU006-001 and DPLKKEU007-001 -> Rerun DPLKKPS143-002 -> Scripting DPLKKPS144-001 until DPLKKPS145-001 08-03-2023 -> Scripting DPLKKEU027-001, DPLKKEU042-001, DPLKKEU045-001 -> Rerun DPLKKPS144-001, DPLKKPS144-002 -> Scripting DPLKKPS152-001 09/03/2023 -> Scripting DPLKKEU026-001, DPLKKEU043-001 until DPLKKEU044-002, DPLKKPS143-002, DPLKKPS149-001, DPLKKPS152-002, DPLKKPS153-001, DPLKKPS153-002
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU006-001 - Keuangan - Transaksi - Entry Penerimaan Teller Perorangan Tambah Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU006-001 - Keuangan - Transaksi - Entry Penerimaan Teller Perorangan Tambah Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D1BF4C-2FC0-432D-8A2F-F86B6EED67CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF1DFC2-7B60-46DE-A935-1599814BC632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>